<commit_message>
lab 3 cpp file
</commit_message>
<xml_diff>
--- a/S23/EESCL/Timesheets/20230309-buziak-timesheet.xlsx
+++ b/S23/EESCL/Timesheets/20230309-buziak-timesheet.xlsx
@@ -1214,9 +1214,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>999720</xdr:colOff>
+      <xdr:colOff>999000</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
+      <xdr:rowOff>131400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1230,7 +1230,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8730720" y="114480"/>
-          <a:ext cx="1416960" cy="808200"/>
+          <a:ext cx="1416240" cy="807480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1253,10 +1253,10 @@
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.13"/>
@@ -1522,10 +1522,10 @@
         <v>0</v>
       </c>
       <c r="E10" s="34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="34" t="n">
         <v>0</v>
@@ -1534,7 +1534,7 @@
       <c r="I10" s="34"/>
       <c r="J10" s="35" t="n">
         <f aca="false">SUM(C10:I10)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L10" s="36"/>
       <c r="M10" s="37"/>
@@ -1766,11 +1766,11 @@
       </c>
       <c r="E19" s="45" t="n">
         <f aca="false">SUM(E10:E18)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="45" t="n">
         <f aca="false">SUM(F10:F18)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="45" t="n">
         <f aca="false">SUM(G10:G18)</f>
@@ -1786,7 +1786,7 @@
       </c>
       <c r="J19" s="45" t="n">
         <f aca="false">SUM(J10:J18)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L19" s="46"/>
       <c r="M19" s="47"/>

</xml_diff>